<commit_message>
Week 11 - Draft
</commit_message>
<xml_diff>
--- a/weekoverzichten/Stage - Week 11.xlsx
+++ b/weekoverzichten/Stage - Week 11.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\sigurd3k\weekoverzichten\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SiVl\Documents\GitHub\sigurd3k.github.io\weekoverzichten\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9390"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9396"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>Maandag</t>
   </si>
@@ -39,13 +39,28 @@
   </si>
   <si>
     <t>Vrijdag</t>
+  </si>
+  <si>
+    <t>Keras Saver fixen</t>
+  </si>
+  <si>
+    <t>Aan document werken</t>
+  </si>
+  <si>
+    <t>Te veel memory van gafische kaart fixen</t>
+  </si>
+  <si>
+    <t>Keras/Tensorflow Saver fixen</t>
+  </si>
+  <si>
+    <t>Keras Saver fixen (het werkt!)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,12 +83,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri Light"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -95,7 +104,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -103,11 +112,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -201,23 +205,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -253,23 +240,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -424,20 +394,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="53.140625" customWidth="1"/>
-    <col min="2" max="2" width="51.28515625" customWidth="1"/>
-    <col min="3" max="3" width="39.7109375" customWidth="1"/>
-    <col min="4" max="4" width="43.85546875" customWidth="1"/>
+    <col min="1" max="1" width="53.109375" customWidth="1"/>
+    <col min="2" max="2" width="51.33203125" customWidth="1"/>
+    <col min="3" max="3" width="39.6640625" customWidth="1"/>
+    <col min="4" max="4" width="43.88671875" customWidth="1"/>
     <col min="5" max="5" width="57" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -454,56 +424,75 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="C4" s="2"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="4"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="4"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>

</xml_diff>